<commit_message>
excel, missatge superar punts
</commit_message>
<xml_diff>
--- a/template.xlsx
+++ b/template.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mdelunag\Downloads\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="990"/>
   </bookViews>
@@ -12,7 +17,7 @@
     <sheet name="Q2" sheetId="3" r:id="rId3"/>
     <sheet name="Assignatures" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -194,7 +199,14 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
+  <dxfs count="7">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFFCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -580,7 +592,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -591,19 +603,19 @@
   <dimension ref="A1:AMK83"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="12.140625" style="1"/>
-    <col min="2" max="2" width="7.42578125" style="1"/>
-    <col min="3" max="3" width="6.5703125" style="1"/>
-    <col min="4" max="53" width="8.140625" style="1"/>
-    <col min="54" max="1025" width="10.5703125" style="1"/>
+    <col min="1" max="1" width="12.1796875" style="1"/>
+    <col min="2" max="2" width="7.453125" style="1"/>
+    <col min="3" max="3" width="6.54296875" style="1"/>
+    <col min="4" max="53" width="8.1796875" style="1"/>
+    <col min="54" max="1025" width="10.54296875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:53" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -813,7 +825,7 @@
         <v/>
       </c>
     </row>
-    <row r="2" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:53" x14ac:dyDescent="0.35">
       <c r="A2" s="6" t="s">
         <v>1</v>
       </c>
@@ -873,7 +885,7 @@
       <c r="AZ2" s="5"/>
       <c r="BA2" s="5"/>
     </row>
-    <row r="3" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:53" x14ac:dyDescent="0.35">
       <c r="A3" s="7" t="s">
         <v>2</v>
       </c>
@@ -1083,7 +1095,7 @@
         <v/>
       </c>
     </row>
-    <row r="4" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:53" x14ac:dyDescent="0.35">
       <c r="A4" s="6" t="s">
         <v>3</v>
       </c>
@@ -1143,7 +1155,7 @@
       <c r="AZ4" s="5"/>
       <c r="BA4" s="5"/>
     </row>
-    <row r="5" spans="1:53" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:53" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="11" t="s">
         <v>4</v>
       </c>
@@ -1204,14 +1216,14 @@
       <c r="AZ5" s="5"/>
       <c r="BA5" s="5"/>
     </row>
-    <row r="6" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:53" x14ac:dyDescent="0.35">
       <c r="A6" s="5"/>
       <c r="B6" s="5" t="str">
         <f t="shared" ref="B6:B37" si="4">IF(A6="","",SUM(D6:BA6))</f>
         <v/>
       </c>
       <c r="C6" s="8" t="str">
-        <f>IF(A6="","",SUMPRODUCT(D6:BA6,D83:BA83))</f>
+        <f>IF(A6="","",SUMPRODUCT(D6:BA6,$D$83:$BA$83))</f>
         <v/>
       </c>
       <c r="D6" s="9"/>
@@ -1265,14 +1277,14 @@
       <c r="AZ6" s="9"/>
       <c r="BA6" s="9"/>
     </row>
-    <row r="7" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:53" x14ac:dyDescent="0.35">
       <c r="A7" s="5"/>
       <c r="B7" s="5" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="C7" s="8" t="str">
-        <f t="shared" ref="C7:C70" si="5">IF(A7="","",SUMPRODUCT(D7:BA7,D84:BA84))</f>
+        <f t="shared" ref="C7:C70" si="5">IF(A7="","",SUMPRODUCT(D7:BA7,$D$83:$BA$83))</f>
         <v/>
       </c>
       <c r="D7" s="9"/>
@@ -1296,7 +1308,7 @@
       <c r="V7" s="9"/>
       <c r="W7" s="9"/>
     </row>
-    <row r="8" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:53" x14ac:dyDescent="0.35">
       <c r="A8" s="5"/>
       <c r="B8" s="5" t="str">
         <f t="shared" si="4"/>
@@ -1327,7 +1339,7 @@
       <c r="V8" s="9"/>
       <c r="W8" s="9"/>
     </row>
-    <row r="9" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:53" x14ac:dyDescent="0.35">
       <c r="A9" s="5"/>
       <c r="B9" s="5" t="str">
         <f t="shared" si="4"/>
@@ -1358,7 +1370,7 @@
       <c r="V9" s="9"/>
       <c r="W9" s="9"/>
     </row>
-    <row r="10" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:53" x14ac:dyDescent="0.35">
       <c r="A10" s="5"/>
       <c r="B10" s="5" t="str">
         <f t="shared" si="4"/>
@@ -1389,7 +1401,7 @@
       <c r="V10" s="9"/>
       <c r="W10" s="9"/>
     </row>
-    <row r="11" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:53" x14ac:dyDescent="0.35">
       <c r="A11" s="5"/>
       <c r="B11" s="5" t="str">
         <f t="shared" si="4"/>
@@ -1420,7 +1432,7 @@
       <c r="V11" s="9"/>
       <c r="W11" s="9"/>
     </row>
-    <row r="12" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:53" x14ac:dyDescent="0.35">
       <c r="A12" s="5"/>
       <c r="B12" s="5" t="str">
         <f t="shared" si="4"/>
@@ -1451,7 +1463,7 @@
       <c r="V12" s="9"/>
       <c r="W12" s="9"/>
     </row>
-    <row r="13" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:53" x14ac:dyDescent="0.35">
       <c r="A13" s="5"/>
       <c r="B13" s="5" t="str">
         <f t="shared" si="4"/>
@@ -1482,7 +1494,7 @@
       <c r="V13" s="9"/>
       <c r="W13" s="9"/>
     </row>
-    <row r="14" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:53" x14ac:dyDescent="0.35">
       <c r="A14" s="5"/>
       <c r="B14" s="5" t="str">
         <f t="shared" si="4"/>
@@ -1513,7 +1525,7 @@
       <c r="V14" s="9"/>
       <c r="W14" s="9"/>
     </row>
-    <row r="15" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:53" x14ac:dyDescent="0.35">
       <c r="A15" s="5"/>
       <c r="B15" s="5" t="str">
         <f t="shared" si="4"/>
@@ -1544,7 +1556,7 @@
       <c r="V15" s="9"/>
       <c r="W15" s="9"/>
     </row>
-    <row r="16" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:53" x14ac:dyDescent="0.35">
       <c r="A16" s="5"/>
       <c r="B16" s="5" t="str">
         <f t="shared" si="4"/>
@@ -1575,7 +1587,7 @@
       <c r="V16" s="9"/>
       <c r="W16" s="9"/>
     </row>
-    <row r="17" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A17" s="5"/>
       <c r="B17" s="5" t="str">
         <f t="shared" si="4"/>
@@ -1606,7 +1618,7 @@
       <c r="V17" s="9"/>
       <c r="W17" s="9"/>
     </row>
-    <row r="18" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A18" s="5"/>
       <c r="B18" s="5" t="str">
         <f t="shared" si="4"/>
@@ -1637,7 +1649,7 @@
       <c r="V18" s="9"/>
       <c r="W18" s="9"/>
     </row>
-    <row r="19" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A19" s="5"/>
       <c r="B19" s="5" t="str">
         <f t="shared" si="4"/>
@@ -1668,7 +1680,7 @@
       <c r="V19" s="9"/>
       <c r="W19" s="9"/>
     </row>
-    <row r="20" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A20" s="5"/>
       <c r="B20" s="5" t="str">
         <f t="shared" si="4"/>
@@ -1699,7 +1711,7 @@
       <c r="V20" s="9"/>
       <c r="W20" s="9"/>
     </row>
-    <row r="21" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A21" s="5"/>
       <c r="B21" s="5" t="str">
         <f t="shared" si="4"/>
@@ -1730,7 +1742,7 @@
       <c r="V21" s="9"/>
       <c r="W21" s="9"/>
     </row>
-    <row r="22" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A22" s="5"/>
       <c r="B22" s="5" t="str">
         <f t="shared" si="4"/>
@@ -1761,7 +1773,7 @@
       <c r="V22" s="9"/>
       <c r="W22" s="9"/>
     </row>
-    <row r="23" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A23" s="5"/>
       <c r="B23" s="5" t="str">
         <f t="shared" si="4"/>
@@ -1792,7 +1804,7 @@
       <c r="V23" s="9"/>
       <c r="W23" s="9"/>
     </row>
-    <row r="24" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A24" s="5"/>
       <c r="B24" s="5" t="str">
         <f t="shared" si="4"/>
@@ -1823,7 +1835,7 @@
       <c r="V24" s="9"/>
       <c r="W24" s="9"/>
     </row>
-    <row r="25" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A25" s="5"/>
       <c r="B25" s="5" t="str">
         <f t="shared" si="4"/>
@@ -1854,7 +1866,7 @@
       <c r="V25" s="9"/>
       <c r="W25" s="9"/>
     </row>
-    <row r="26" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A26" s="5"/>
       <c r="B26" s="5" t="str">
         <f t="shared" si="4"/>
@@ -1885,7 +1897,7 @@
       <c r="V26" s="9"/>
       <c r="W26" s="9"/>
     </row>
-    <row r="27" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A27" s="5"/>
       <c r="B27" s="5" t="str">
         <f t="shared" si="4"/>
@@ -1916,7 +1928,7 @@
       <c r="V27" s="9"/>
       <c r="W27" s="9"/>
     </row>
-    <row r="28" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A28" s="5"/>
       <c r="B28" s="5" t="str">
         <f t="shared" si="4"/>
@@ -1947,7 +1959,7 @@
       <c r="V28" s="9"/>
       <c r="W28" s="9"/>
     </row>
-    <row r="29" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A29" s="5"/>
       <c r="B29" s="5" t="str">
         <f t="shared" si="4"/>
@@ -1978,7 +1990,7 @@
       <c r="V29" s="9"/>
       <c r="W29" s="9"/>
     </row>
-    <row r="30" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A30" s="5"/>
       <c r="B30" s="5" t="str">
         <f t="shared" si="4"/>
@@ -2009,7 +2021,7 @@
       <c r="V30" s="9"/>
       <c r="W30" s="9"/>
     </row>
-    <row r="31" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A31" s="5"/>
       <c r="B31" s="5" t="str">
         <f t="shared" si="4"/>
@@ -2040,7 +2052,7 @@
       <c r="V31" s="9"/>
       <c r="W31" s="9"/>
     </row>
-    <row r="32" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A32" s="5"/>
       <c r="B32" s="5" t="str">
         <f t="shared" si="4"/>
@@ -2071,7 +2083,7 @@
       <c r="V32" s="9"/>
       <c r="W32" s="9"/>
     </row>
-    <row r="33" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A33" s="5"/>
       <c r="B33" s="5" t="str">
         <f t="shared" si="4"/>
@@ -2102,7 +2114,7 @@
       <c r="V33" s="9"/>
       <c r="W33" s="9"/>
     </row>
-    <row r="34" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A34" s="5"/>
       <c r="B34" s="5" t="str">
         <f t="shared" si="4"/>
@@ -2133,7 +2145,7 @@
       <c r="V34" s="9"/>
       <c r="W34" s="9"/>
     </row>
-    <row r="35" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A35" s="5"/>
       <c r="B35" s="5" t="str">
         <f t="shared" si="4"/>
@@ -2164,7 +2176,7 @@
       <c r="V35" s="9"/>
       <c r="W35" s="9"/>
     </row>
-    <row r="36" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A36" s="5"/>
       <c r="B36" s="5" t="str">
         <f t="shared" si="4"/>
@@ -2195,7 +2207,7 @@
       <c r="V36" s="9"/>
       <c r="W36" s="9"/>
     </row>
-    <row r="37" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A37" s="5"/>
       <c r="B37" s="5" t="str">
         <f t="shared" si="4"/>
@@ -2226,7 +2238,7 @@
       <c r="V37" s="9"/>
       <c r="W37" s="9"/>
     </row>
-    <row r="38" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A38" s="5"/>
       <c r="B38" s="5" t="str">
         <f t="shared" ref="B38:B69" si="6">IF(A38="","",SUM(D38:BA38))</f>
@@ -2257,7 +2269,7 @@
       <c r="V38" s="9"/>
       <c r="W38" s="9"/>
     </row>
-    <row r="39" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A39" s="5"/>
       <c r="B39" s="5" t="str">
         <f t="shared" si="6"/>
@@ -2288,7 +2300,7 @@
       <c r="V39" s="9"/>
       <c r="W39" s="9"/>
     </row>
-    <row r="40" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A40" s="5"/>
       <c r="B40" s="5" t="str">
         <f t="shared" si="6"/>
@@ -2319,7 +2331,7 @@
       <c r="V40" s="9"/>
       <c r="W40" s="9"/>
     </row>
-    <row r="41" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A41" s="5"/>
       <c r="B41" s="5" t="str">
         <f t="shared" si="6"/>
@@ -2350,7 +2362,7 @@
       <c r="V41" s="9"/>
       <c r="W41" s="9"/>
     </row>
-    <row r="42" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A42" s="5"/>
       <c r="B42" s="5" t="str">
         <f t="shared" si="6"/>
@@ -2381,7 +2393,7 @@
       <c r="V42" s="9"/>
       <c r="W42" s="9"/>
     </row>
-    <row r="43" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A43" s="5"/>
       <c r="B43" s="5" t="str">
         <f t="shared" si="6"/>
@@ -2412,7 +2424,7 @@
       <c r="V43" s="9"/>
       <c r="W43" s="9"/>
     </row>
-    <row r="44" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A44" s="5"/>
       <c r="B44" s="5" t="str">
         <f t="shared" si="6"/>
@@ -2443,7 +2455,7 @@
       <c r="V44" s="9"/>
       <c r="W44" s="9"/>
     </row>
-    <row r="45" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A45" s="5"/>
       <c r="B45" s="5" t="str">
         <f t="shared" si="6"/>
@@ -2474,7 +2486,7 @@
       <c r="V45" s="9"/>
       <c r="W45" s="9"/>
     </row>
-    <row r="46" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A46" s="5"/>
       <c r="B46" s="5" t="str">
         <f t="shared" si="6"/>
@@ -2505,7 +2517,7 @@
       <c r="V46" s="9"/>
       <c r="W46" s="9"/>
     </row>
-    <row r="47" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A47" s="5"/>
       <c r="B47" s="5" t="str">
         <f t="shared" si="6"/>
@@ -2536,7 +2548,7 @@
       <c r="V47" s="9"/>
       <c r="W47" s="9"/>
     </row>
-    <row r="48" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A48" s="5"/>
       <c r="B48" s="5" t="str">
         <f t="shared" si="6"/>
@@ -2567,7 +2579,7 @@
       <c r="V48" s="9"/>
       <c r="W48" s="9"/>
     </row>
-    <row r="49" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A49" s="5"/>
       <c r="B49" s="5" t="str">
         <f t="shared" si="6"/>
@@ -2598,7 +2610,7 @@
       <c r="V49" s="9"/>
       <c r="W49" s="9"/>
     </row>
-    <row r="50" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A50" s="5"/>
       <c r="B50" s="5" t="str">
         <f t="shared" si="6"/>
@@ -2629,7 +2641,7 @@
       <c r="V50" s="9"/>
       <c r="W50" s="9"/>
     </row>
-    <row r="51" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A51" s="5"/>
       <c r="B51" s="5" t="str">
         <f t="shared" si="6"/>
@@ -2660,7 +2672,7 @@
       <c r="V51" s="9"/>
       <c r="W51" s="9"/>
     </row>
-    <row r="52" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A52" s="5"/>
       <c r="B52" s="5" t="str">
         <f t="shared" si="6"/>
@@ -2691,7 +2703,7 @@
       <c r="V52" s="9"/>
       <c r="W52" s="9"/>
     </row>
-    <row r="53" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A53" s="5"/>
       <c r="B53" s="5" t="str">
         <f t="shared" si="6"/>
@@ -2722,7 +2734,7 @@
       <c r="V53" s="9"/>
       <c r="W53" s="9"/>
     </row>
-    <row r="54" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A54" s="5"/>
       <c r="B54" s="5" t="str">
         <f t="shared" si="6"/>
@@ -2753,7 +2765,7 @@
       <c r="V54" s="9"/>
       <c r="W54" s="9"/>
     </row>
-    <row r="55" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A55" s="5"/>
       <c r="B55" s="5" t="str">
         <f t="shared" si="6"/>
@@ -2784,7 +2796,7 @@
       <c r="V55" s="9"/>
       <c r="W55" s="9"/>
     </row>
-    <row r="56" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A56" s="5"/>
       <c r="B56" s="5" t="str">
         <f t="shared" si="6"/>
@@ -2815,7 +2827,7 @@
       <c r="V56" s="9"/>
       <c r="W56" s="9"/>
     </row>
-    <row r="57" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A57" s="5"/>
       <c r="B57" s="5" t="str">
         <f t="shared" si="6"/>
@@ -2846,7 +2858,7 @@
       <c r="V57" s="9"/>
       <c r="W57" s="9"/>
     </row>
-    <row r="58" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A58" s="5"/>
       <c r="B58" s="5" t="str">
         <f t="shared" si="6"/>
@@ -2877,7 +2889,7 @@
       <c r="V58" s="9"/>
       <c r="W58" s="9"/>
     </row>
-    <row r="59" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A59" s="5"/>
       <c r="B59" s="5" t="str">
         <f t="shared" si="6"/>
@@ -2908,7 +2920,7 @@
       <c r="V59" s="9"/>
       <c r="W59" s="9"/>
     </row>
-    <row r="60" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A60" s="5"/>
       <c r="B60" s="5" t="str">
         <f t="shared" si="6"/>
@@ -2939,7 +2951,7 @@
       <c r="V60" s="9"/>
       <c r="W60" s="9"/>
     </row>
-    <row r="61" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A61" s="5"/>
       <c r="B61" s="5" t="str">
         <f t="shared" si="6"/>
@@ -2970,7 +2982,7 @@
       <c r="V61" s="9"/>
       <c r="W61" s="9"/>
     </row>
-    <row r="62" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A62" s="5"/>
       <c r="B62" s="5" t="str">
         <f t="shared" si="6"/>
@@ -3001,7 +3013,7 @@
       <c r="V62" s="9"/>
       <c r="W62" s="9"/>
     </row>
-    <row r="63" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A63" s="5"/>
       <c r="B63" s="5" t="str">
         <f t="shared" si="6"/>
@@ -3032,7 +3044,7 @@
       <c r="V63" s="9"/>
       <c r="W63" s="9"/>
     </row>
-    <row r="64" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A64" s="5"/>
       <c r="B64" s="5" t="str">
         <f t="shared" si="6"/>
@@ -3063,7 +3075,7 @@
       <c r="V64" s="9"/>
       <c r="W64" s="9"/>
     </row>
-    <row r="65" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A65" s="5"/>
       <c r="B65" s="5" t="str">
         <f t="shared" si="6"/>
@@ -3094,7 +3106,7 @@
       <c r="V65" s="9"/>
       <c r="W65" s="9"/>
     </row>
-    <row r="66" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A66" s="5"/>
       <c r="B66" s="5" t="str">
         <f t="shared" si="6"/>
@@ -3125,7 +3137,7 @@
       <c r="V66" s="9"/>
       <c r="W66" s="9"/>
     </row>
-    <row r="67" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A67" s="5"/>
       <c r="B67" s="5" t="str">
         <f t="shared" si="6"/>
@@ -3156,7 +3168,7 @@
       <c r="V67" s="9"/>
       <c r="W67" s="9"/>
     </row>
-    <row r="68" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A68" s="5"/>
       <c r="B68" s="5" t="str">
         <f t="shared" si="6"/>
@@ -3187,7 +3199,7 @@
       <c r="V68" s="9"/>
       <c r="W68" s="9"/>
     </row>
-    <row r="69" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A69" s="5"/>
       <c r="B69" s="5" t="str">
         <f t="shared" si="6"/>
@@ -3218,7 +3230,7 @@
       <c r="V69" s="9"/>
       <c r="W69" s="9"/>
     </row>
-    <row r="70" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A70" s="5"/>
       <c r="B70" s="5" t="str">
         <f t="shared" ref="B70:B81" si="7">IF(A70="","",SUM(D70:BA70))</f>
@@ -3229,18 +3241,18 @@
         <v/>
       </c>
     </row>
-    <row r="71" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A71" s="5"/>
       <c r="B71" s="5" t="str">
         <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="C71" s="8" t="str">
-        <f t="shared" ref="C71:C82" si="8">IF(A71="","",SUMPRODUCT(D71:BA71,D148:BA148))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="72" spans="1:23" x14ac:dyDescent="0.25">
+        <f t="shared" ref="C71:C82" si="8">IF(A71="","",SUMPRODUCT(D71:BA71,$D$83:$BA$83))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="72" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A72" s="5"/>
       <c r="B72" s="5" t="str">
         <f t="shared" si="7"/>
@@ -3251,7 +3263,7 @@
         <v/>
       </c>
     </row>
-    <row r="73" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A73" s="5"/>
       <c r="B73" s="5" t="str">
         <f t="shared" si="7"/>
@@ -3262,7 +3274,7 @@
         <v/>
       </c>
     </row>
-    <row r="74" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A74" s="5"/>
       <c r="B74" s="5" t="str">
         <f t="shared" si="7"/>
@@ -3273,7 +3285,7 @@
         <v/>
       </c>
     </row>
-    <row r="75" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A75" s="5"/>
       <c r="B75" s="5" t="str">
         <f t="shared" si="7"/>
@@ -3284,7 +3296,7 @@
         <v/>
       </c>
     </row>
-    <row r="76" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A76" s="5"/>
       <c r="B76" s="5" t="str">
         <f t="shared" si="7"/>
@@ -3295,7 +3307,7 @@
         <v/>
       </c>
     </row>
-    <row r="77" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A77" s="5"/>
       <c r="B77" s="5" t="str">
         <f t="shared" si="7"/>
@@ -3306,7 +3318,7 @@
         <v/>
       </c>
     </row>
-    <row r="78" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A78" s="5"/>
       <c r="B78" s="5" t="str">
         <f t="shared" si="7"/>
@@ -3317,7 +3329,7 @@
         <v/>
       </c>
     </row>
-    <row r="79" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A79" s="5"/>
       <c r="B79" s="5" t="str">
         <f t="shared" si="7"/>
@@ -3328,7 +3340,7 @@
         <v/>
       </c>
     </row>
-    <row r="80" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A80" s="5"/>
       <c r="B80" s="5" t="str">
         <f t="shared" si="7"/>
@@ -3339,7 +3351,7 @@
         <v/>
       </c>
     </row>
-    <row r="81" spans="1:97" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:97" x14ac:dyDescent="0.35">
       <c r="A81" s="5"/>
       <c r="B81" s="5" t="str">
         <f t="shared" si="7"/>
@@ -3350,13 +3362,13 @@
         <v/>
       </c>
     </row>
-    <row r="82" spans="1:97" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:97" x14ac:dyDescent="0.35">
       <c r="C82" s="8" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
     </row>
-    <row r="83" spans="1:97" hidden="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:97" hidden="1" x14ac:dyDescent="0.35">
       <c r="A83" s="1" t="s">
         <v>11</v>
       </c>
@@ -3739,12 +3751,12 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A6:A90 D5:CD5">
-    <cfRule type="notContainsBlanks" dxfId="5" priority="3">
+    <cfRule type="notContainsBlanks" dxfId="6" priority="3">
       <formula>LEN(TRIM(A5))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B6:C88">
-    <cfRule type="notContainsBlanks" dxfId="4" priority="1">
+    <cfRule type="notContainsBlanks" dxfId="5" priority="1">
       <formula>LEN(TRIM(B6))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3761,12 +3773,12 @@
       <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1025" width="8.7109375" style="1"/>
+    <col min="1" max="1025" width="8.7265625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:53" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -3976,7 +3988,7 @@
         <v/>
       </c>
     </row>
-    <row r="2" spans="1:53" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:53" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="6" t="s">
         <v>1</v>
       </c>
@@ -4036,7 +4048,7 @@
       <c r="AZ2" s="5"/>
       <c r="BA2" s="5"/>
     </row>
-    <row r="3" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:53" x14ac:dyDescent="0.35">
       <c r="A3" s="7" t="s">
         <v>2</v>
       </c>
@@ -4246,7 +4258,7 @@
         <v/>
       </c>
     </row>
-    <row r="4" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:53" x14ac:dyDescent="0.35">
       <c r="A4" s="6" t="s">
         <v>3</v>
       </c>
@@ -4306,7 +4318,7 @@
       <c r="AZ4" s="5"/>
       <c r="BA4" s="5"/>
     </row>
-    <row r="5" spans="1:53" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:53" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="11" t="s">
         <v>4</v>
       </c>
@@ -4367,7 +4379,7 @@
       <c r="AZ5" s="5"/>
       <c r="BA5" s="5"/>
     </row>
-    <row r="6" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:53" x14ac:dyDescent="0.35">
       <c r="A6" s="5"/>
       <c r="B6" s="5" t="str">
         <f t="shared" ref="B6:B69" si="2">IF(A6="","",SUM(D6:BA6))</f>
@@ -4428,7 +4440,7 @@
       <c r="AZ6" s="9"/>
       <c r="BA6" s="9"/>
     </row>
-    <row r="7" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:53" x14ac:dyDescent="0.35">
       <c r="A7" s="5"/>
       <c r="B7" s="5" t="str">
         <f t="shared" si="2"/>
@@ -4459,7 +4471,7 @@
       <c r="V7" s="9"/>
       <c r="W7" s="9"/>
     </row>
-    <row r="8" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:53" x14ac:dyDescent="0.35">
       <c r="A8" s="5"/>
       <c r="B8" s="5" t="str">
         <f t="shared" si="2"/>
@@ -4490,7 +4502,7 @@
       <c r="V8" s="9"/>
       <c r="W8" s="9"/>
     </row>
-    <row r="9" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:53" x14ac:dyDescent="0.35">
       <c r="A9" s="5"/>
       <c r="B9" s="5" t="str">
         <f t="shared" si="2"/>
@@ -4521,7 +4533,7 @@
       <c r="V9" s="9"/>
       <c r="W9" s="9"/>
     </row>
-    <row r="10" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:53" x14ac:dyDescent="0.35">
       <c r="A10" s="5"/>
       <c r="B10" s="5" t="str">
         <f t="shared" si="2"/>
@@ -4552,7 +4564,7 @@
       <c r="V10" s="9"/>
       <c r="W10" s="9"/>
     </row>
-    <row r="11" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:53" x14ac:dyDescent="0.35">
       <c r="A11" s="5"/>
       <c r="B11" s="5" t="str">
         <f t="shared" si="2"/>
@@ -4583,7 +4595,7 @@
       <c r="V11" s="9"/>
       <c r="W11" s="9"/>
     </row>
-    <row r="12" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:53" x14ac:dyDescent="0.35">
       <c r="A12" s="5"/>
       <c r="B12" s="5" t="str">
         <f t="shared" si="2"/>
@@ -4614,7 +4626,7 @@
       <c r="V12" s="9"/>
       <c r="W12" s="9"/>
     </row>
-    <row r="13" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:53" x14ac:dyDescent="0.35">
       <c r="A13" s="5"/>
       <c r="B13" s="5" t="str">
         <f t="shared" si="2"/>
@@ -4645,7 +4657,7 @@
       <c r="V13" s="9"/>
       <c r="W13" s="9"/>
     </row>
-    <row r="14" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:53" x14ac:dyDescent="0.35">
       <c r="A14" s="5"/>
       <c r="B14" s="5" t="str">
         <f t="shared" si="2"/>
@@ -4676,7 +4688,7 @@
       <c r="V14" s="9"/>
       <c r="W14" s="9"/>
     </row>
-    <row r="15" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:53" x14ac:dyDescent="0.35">
       <c r="A15" s="5"/>
       <c r="B15" s="5" t="str">
         <f t="shared" si="2"/>
@@ -4707,7 +4719,7 @@
       <c r="V15" s="9"/>
       <c r="W15" s="9"/>
     </row>
-    <row r="16" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:53" x14ac:dyDescent="0.35">
       <c r="A16" s="5"/>
       <c r="B16" s="5" t="str">
         <f t="shared" si="2"/>
@@ -4738,7 +4750,7 @@
       <c r="V16" s="9"/>
       <c r="W16" s="9"/>
     </row>
-    <row r="17" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A17" s="5"/>
       <c r="B17" s="5" t="str">
         <f t="shared" si="2"/>
@@ -4769,7 +4781,7 @@
       <c r="V17" s="9"/>
       <c r="W17" s="9"/>
     </row>
-    <row r="18" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A18" s="5"/>
       <c r="B18" s="5" t="str">
         <f t="shared" si="2"/>
@@ -4800,7 +4812,7 @@
       <c r="V18" s="9"/>
       <c r="W18" s="9"/>
     </row>
-    <row r="19" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A19" s="5"/>
       <c r="B19" s="5" t="str">
         <f t="shared" si="2"/>
@@ -4831,7 +4843,7 @@
       <c r="V19" s="9"/>
       <c r="W19" s="9"/>
     </row>
-    <row r="20" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A20" s="5"/>
       <c r="B20" s="5" t="str">
         <f t="shared" si="2"/>
@@ -4862,7 +4874,7 @@
       <c r="V20" s="9"/>
       <c r="W20" s="9"/>
     </row>
-    <row r="21" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A21" s="5"/>
       <c r="B21" s="5" t="str">
         <f t="shared" si="2"/>
@@ -4893,7 +4905,7 @@
       <c r="V21" s="9"/>
       <c r="W21" s="9"/>
     </row>
-    <row r="22" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A22" s="5"/>
       <c r="B22" s="5" t="str">
         <f t="shared" si="2"/>
@@ -4924,7 +4936,7 @@
       <c r="V22" s="9"/>
       <c r="W22" s="9"/>
     </row>
-    <row r="23" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A23" s="5"/>
       <c r="B23" s="5" t="str">
         <f t="shared" si="2"/>
@@ -4955,7 +4967,7 @@
       <c r="V23" s="9"/>
       <c r="W23" s="9"/>
     </row>
-    <row r="24" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A24" s="5"/>
       <c r="B24" s="5" t="str">
         <f t="shared" si="2"/>
@@ -4986,7 +4998,7 @@
       <c r="V24" s="9"/>
       <c r="W24" s="9"/>
     </row>
-    <row r="25" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A25" s="5"/>
       <c r="B25" s="5" t="str">
         <f t="shared" si="2"/>
@@ -5017,7 +5029,7 @@
       <c r="V25" s="9"/>
       <c r="W25" s="9"/>
     </row>
-    <row r="26" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A26" s="5"/>
       <c r="B26" s="5" t="str">
         <f t="shared" si="2"/>
@@ -5048,7 +5060,7 @@
       <c r="V26" s="9"/>
       <c r="W26" s="9"/>
     </row>
-    <row r="27" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A27" s="5"/>
       <c r="B27" s="5" t="str">
         <f t="shared" si="2"/>
@@ -5079,7 +5091,7 @@
       <c r="V27" s="9"/>
       <c r="W27" s="9"/>
     </row>
-    <row r="28" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A28" s="5"/>
       <c r="B28" s="5" t="str">
         <f t="shared" si="2"/>
@@ -5110,7 +5122,7 @@
       <c r="V28" s="9"/>
       <c r="W28" s="9"/>
     </row>
-    <row r="29" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A29" s="5"/>
       <c r="B29" s="5" t="str">
         <f t="shared" si="2"/>
@@ -5141,7 +5153,7 @@
       <c r="V29" s="9"/>
       <c r="W29" s="9"/>
     </row>
-    <row r="30" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A30" s="5"/>
       <c r="B30" s="5" t="str">
         <f t="shared" si="2"/>
@@ -5172,7 +5184,7 @@
       <c r="V30" s="9"/>
       <c r="W30" s="9"/>
     </row>
-    <row r="31" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A31" s="5"/>
       <c r="B31" s="5" t="str">
         <f t="shared" si="2"/>
@@ -5203,7 +5215,7 @@
       <c r="V31" s="9"/>
       <c r="W31" s="9"/>
     </row>
-    <row r="32" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A32" s="5"/>
       <c r="B32" s="5" t="str">
         <f t="shared" si="2"/>
@@ -5234,7 +5246,7 @@
       <c r="V32" s="9"/>
       <c r="W32" s="9"/>
     </row>
-    <row r="33" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A33" s="5"/>
       <c r="B33" s="5" t="str">
         <f t="shared" si="2"/>
@@ -5265,7 +5277,7 @@
       <c r="V33" s="9"/>
       <c r="W33" s="9"/>
     </row>
-    <row r="34" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A34" s="5"/>
       <c r="B34" s="5" t="str">
         <f t="shared" si="2"/>
@@ -5296,7 +5308,7 @@
       <c r="V34" s="9"/>
       <c r="W34" s="9"/>
     </row>
-    <row r="35" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A35" s="5"/>
       <c r="B35" s="5" t="str">
         <f t="shared" si="2"/>
@@ -5327,7 +5339,7 @@
       <c r="V35" s="9"/>
       <c r="W35" s="9"/>
     </row>
-    <row r="36" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A36" s="5"/>
       <c r="B36" s="5" t="str">
         <f t="shared" si="2"/>
@@ -5358,7 +5370,7 @@
       <c r="V36" s="9"/>
       <c r="W36" s="9"/>
     </row>
-    <row r="37" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A37" s="5"/>
       <c r="B37" s="5" t="str">
         <f t="shared" si="2"/>
@@ -5389,7 +5401,7 @@
       <c r="V37" s="9"/>
       <c r="W37" s="9"/>
     </row>
-    <row r="38" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A38" s="5"/>
       <c r="B38" s="5" t="str">
         <f t="shared" si="2"/>
@@ -5420,7 +5432,7 @@
       <c r="V38" s="9"/>
       <c r="W38" s="9"/>
     </row>
-    <row r="39" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A39" s="5"/>
       <c r="B39" s="5" t="str">
         <f t="shared" si="2"/>
@@ -5451,7 +5463,7 @@
       <c r="V39" s="9"/>
       <c r="W39" s="9"/>
     </row>
-    <row r="40" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A40" s="5"/>
       <c r="B40" s="5" t="str">
         <f t="shared" si="2"/>
@@ -5482,7 +5494,7 @@
       <c r="V40" s="9"/>
       <c r="W40" s="9"/>
     </row>
-    <row r="41" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A41" s="5"/>
       <c r="B41" s="5" t="str">
         <f t="shared" si="2"/>
@@ -5513,7 +5525,7 @@
       <c r="V41" s="9"/>
       <c r="W41" s="9"/>
     </row>
-    <row r="42" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A42" s="5"/>
       <c r="B42" s="5" t="str">
         <f t="shared" si="2"/>
@@ -5544,7 +5556,7 @@
       <c r="V42" s="9"/>
       <c r="W42" s="9"/>
     </row>
-    <row r="43" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A43" s="5"/>
       <c r="B43" s="5" t="str">
         <f t="shared" si="2"/>
@@ -5575,7 +5587,7 @@
       <c r="V43" s="9"/>
       <c r="W43" s="9"/>
     </row>
-    <row r="44" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A44" s="5"/>
       <c r="B44" s="5" t="str">
         <f t="shared" si="2"/>
@@ -5606,7 +5618,7 @@
       <c r="V44" s="9"/>
       <c r="W44" s="9"/>
     </row>
-    <row r="45" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A45" s="5"/>
       <c r="B45" s="5" t="str">
         <f t="shared" si="2"/>
@@ -5637,7 +5649,7 @@
       <c r="V45" s="9"/>
       <c r="W45" s="9"/>
     </row>
-    <row r="46" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A46" s="5"/>
       <c r="B46" s="5" t="str">
         <f t="shared" si="2"/>
@@ -5668,7 +5680,7 @@
       <c r="V46" s="9"/>
       <c r="W46" s="9"/>
     </row>
-    <row r="47" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A47" s="5"/>
       <c r="B47" s="5" t="str">
         <f t="shared" si="2"/>
@@ -5699,7 +5711,7 @@
       <c r="V47" s="9"/>
       <c r="W47" s="9"/>
     </row>
-    <row r="48" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A48" s="5"/>
       <c r="B48" s="5" t="str">
         <f t="shared" si="2"/>
@@ -5730,7 +5742,7 @@
       <c r="V48" s="9"/>
       <c r="W48" s="9"/>
     </row>
-    <row r="49" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A49" s="5"/>
       <c r="B49" s="5" t="str">
         <f t="shared" si="2"/>
@@ -5761,7 +5773,7 @@
       <c r="V49" s="9"/>
       <c r="W49" s="9"/>
     </row>
-    <row r="50" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A50" s="5"/>
       <c r="B50" s="5" t="str">
         <f t="shared" si="2"/>
@@ -5792,7 +5804,7 @@
       <c r="V50" s="9"/>
       <c r="W50" s="9"/>
     </row>
-    <row r="51" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A51" s="5"/>
       <c r="B51" s="5" t="str">
         <f t="shared" si="2"/>
@@ -5823,7 +5835,7 @@
       <c r="V51" s="9"/>
       <c r="W51" s="9"/>
     </row>
-    <row r="52" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A52" s="5"/>
       <c r="B52" s="5" t="str">
         <f t="shared" si="2"/>
@@ -5854,7 +5866,7 @@
       <c r="V52" s="9"/>
       <c r="W52" s="9"/>
     </row>
-    <row r="53" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A53" s="5"/>
       <c r="B53" s="5" t="str">
         <f t="shared" si="2"/>
@@ -5885,7 +5897,7 @@
       <c r="V53" s="9"/>
       <c r="W53" s="9"/>
     </row>
-    <row r="54" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A54" s="5"/>
       <c r="B54" s="5" t="str">
         <f t="shared" si="2"/>
@@ -5916,7 +5928,7 @@
       <c r="V54" s="9"/>
       <c r="W54" s="9"/>
     </row>
-    <row r="55" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A55" s="5"/>
       <c r="B55" s="5" t="str">
         <f t="shared" si="2"/>
@@ -5947,7 +5959,7 @@
       <c r="V55" s="9"/>
       <c r="W55" s="9"/>
     </row>
-    <row r="56" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A56" s="5"/>
       <c r="B56" s="5" t="str">
         <f t="shared" si="2"/>
@@ -5978,7 +5990,7 @@
       <c r="V56" s="9"/>
       <c r="W56" s="9"/>
     </row>
-    <row r="57" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A57" s="5"/>
       <c r="B57" s="5" t="str">
         <f t="shared" si="2"/>
@@ -6009,7 +6021,7 @@
       <c r="V57" s="9"/>
       <c r="W57" s="9"/>
     </row>
-    <row r="58" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A58" s="5"/>
       <c r="B58" s="5" t="str">
         <f t="shared" si="2"/>
@@ -6040,7 +6052,7 @@
       <c r="V58" s="9"/>
       <c r="W58" s="9"/>
     </row>
-    <row r="59" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A59" s="5"/>
       <c r="B59" s="5" t="str">
         <f t="shared" si="2"/>
@@ -6071,7 +6083,7 @@
       <c r="V59" s="9"/>
       <c r="W59" s="9"/>
     </row>
-    <row r="60" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A60" s="5"/>
       <c r="B60" s="5" t="str">
         <f t="shared" si="2"/>
@@ -6102,7 +6114,7 @@
       <c r="V60" s="9"/>
       <c r="W60" s="9"/>
     </row>
-    <row r="61" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A61" s="5"/>
       <c r="B61" s="5" t="str">
         <f t="shared" si="2"/>
@@ -6133,7 +6145,7 @@
       <c r="V61" s="9"/>
       <c r="W61" s="9"/>
     </row>
-    <row r="62" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A62" s="5"/>
       <c r="B62" s="5" t="str">
         <f t="shared" si="2"/>
@@ -6164,7 +6176,7 @@
       <c r="V62" s="9"/>
       <c r="W62" s="9"/>
     </row>
-    <row r="63" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A63" s="5"/>
       <c r="B63" s="5" t="str">
         <f t="shared" si="2"/>
@@ -6195,7 +6207,7 @@
       <c r="V63" s="9"/>
       <c r="W63" s="9"/>
     </row>
-    <row r="64" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A64" s="5"/>
       <c r="B64" s="5" t="str">
         <f t="shared" si="2"/>
@@ -6226,7 +6238,7 @@
       <c r="V64" s="9"/>
       <c r="W64" s="9"/>
     </row>
-    <row r="65" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A65" s="5"/>
       <c r="B65" s="5" t="str">
         <f t="shared" si="2"/>
@@ -6257,7 +6269,7 @@
       <c r="V65" s="9"/>
       <c r="W65" s="9"/>
     </row>
-    <row r="66" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A66" s="5"/>
       <c r="B66" s="5" t="str">
         <f t="shared" si="2"/>
@@ -6288,7 +6300,7 @@
       <c r="V66" s="9"/>
       <c r="W66" s="9"/>
     </row>
-    <row r="67" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A67" s="5"/>
       <c r="B67" s="5" t="str">
         <f t="shared" si="2"/>
@@ -6319,7 +6331,7 @@
       <c r="V67" s="9"/>
       <c r="W67" s="9"/>
     </row>
-    <row r="68" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A68" s="5"/>
       <c r="B68" s="5" t="str">
         <f t="shared" si="2"/>
@@ -6350,7 +6362,7 @@
       <c r="V68" s="9"/>
       <c r="W68" s="9"/>
     </row>
-    <row r="69" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A69" s="5"/>
       <c r="B69" s="5" t="str">
         <f t="shared" si="2"/>
@@ -6381,7 +6393,7 @@
       <c r="V69" s="9"/>
       <c r="W69" s="9"/>
     </row>
-    <row r="70" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A70" s="5"/>
       <c r="B70" s="5" t="str">
         <f t="shared" ref="B70:B81" si="4">IF(A70="","",SUM(D70:BA70))</f>
@@ -6392,7 +6404,7 @@
         <v/>
       </c>
     </row>
-    <row r="71" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A71" s="5"/>
       <c r="B71" s="5" t="str">
         <f t="shared" si="4"/>
@@ -6403,7 +6415,7 @@
         <v/>
       </c>
     </row>
-    <row r="72" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A72" s="5"/>
       <c r="B72" s="5" t="str">
         <f t="shared" si="4"/>
@@ -6414,7 +6426,7 @@
         <v/>
       </c>
     </row>
-    <row r="73" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A73" s="5"/>
       <c r="B73" s="5" t="str">
         <f t="shared" si="4"/>
@@ -6425,7 +6437,7 @@
         <v/>
       </c>
     </row>
-    <row r="74" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A74" s="5"/>
       <c r="B74" s="5" t="str">
         <f t="shared" si="4"/>
@@ -6436,7 +6448,7 @@
         <v/>
       </c>
     </row>
-    <row r="75" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A75" s="5"/>
       <c r="B75" s="5" t="str">
         <f t="shared" si="4"/>
@@ -6447,7 +6459,7 @@
         <v/>
       </c>
     </row>
-    <row r="76" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A76" s="5"/>
       <c r="B76" s="5" t="str">
         <f t="shared" si="4"/>
@@ -6458,7 +6470,7 @@
         <v/>
       </c>
     </row>
-    <row r="77" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A77" s="5"/>
       <c r="B77" s="5" t="str">
         <f t="shared" si="4"/>
@@ -6469,7 +6481,7 @@
         <v/>
       </c>
     </row>
-    <row r="78" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A78" s="5"/>
       <c r="B78" s="5" t="str">
         <f t="shared" si="4"/>
@@ -6480,7 +6492,7 @@
         <v/>
       </c>
     </row>
-    <row r="79" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A79" s="5"/>
       <c r="B79" s="5" t="str">
         <f t="shared" si="4"/>
@@ -6491,7 +6503,7 @@
         <v/>
       </c>
     </row>
-    <row r="80" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A80" s="5"/>
       <c r="B80" s="5" t="str">
         <f t="shared" si="4"/>
@@ -6502,7 +6514,7 @@
         <v/>
       </c>
     </row>
-    <row r="81" spans="1:97" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:97" x14ac:dyDescent="0.35">
       <c r="A81" s="5"/>
       <c r="B81" s="5" t="str">
         <f t="shared" si="4"/>
@@ -6513,13 +6525,13 @@
         <v/>
       </c>
     </row>
-    <row r="82" spans="1:97" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:97" x14ac:dyDescent="0.35">
       <c r="C82" s="8" t="str">
         <f t="shared" si="5"/>
         <v/>
       </c>
     </row>
-    <row r="83" spans="1:97" hidden="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:97" hidden="1" x14ac:dyDescent="0.35">
       <c r="A83" s="1" t="s">
         <v>11</v>
       </c>
@@ -6902,12 +6914,12 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A6:A90 D5:CD5">
-    <cfRule type="notContainsBlanks" dxfId="3" priority="2">
+    <cfRule type="notContainsBlanks" dxfId="4" priority="2">
       <formula>LEN(TRIM(A5))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B6:C88">
-    <cfRule type="notContainsBlanks" dxfId="2" priority="1">
+    <cfRule type="notContainsBlanks" dxfId="3" priority="1">
       <formula>LEN(TRIM(B6))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -6924,12 +6936,12 @@
       <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1025" width="8.7109375" style="1"/>
+    <col min="1" max="1025" width="8.7265625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:53" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -7139,7 +7151,7 @@
         <v/>
       </c>
     </row>
-    <row r="2" spans="1:53" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:53" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="6" t="s">
         <v>1</v>
       </c>
@@ -7199,7 +7211,7 @@
       <c r="AZ2" s="5"/>
       <c r="BA2" s="5"/>
     </row>
-    <row r="3" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:53" x14ac:dyDescent="0.35">
       <c r="A3" s="7" t="s">
         <v>2</v>
       </c>
@@ -7409,7 +7421,7 @@
         <v/>
       </c>
     </row>
-    <row r="4" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:53" x14ac:dyDescent="0.35">
       <c r="A4" s="6" t="s">
         <v>3</v>
       </c>
@@ -7469,7 +7481,7 @@
       <c r="AZ4" s="5"/>
       <c r="BA4" s="5"/>
     </row>
-    <row r="5" spans="1:53" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:53" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="11" t="s">
         <v>4</v>
       </c>
@@ -7530,7 +7542,7 @@
       <c r="AZ5" s="5"/>
       <c r="BA5" s="5"/>
     </row>
-    <row r="6" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:53" x14ac:dyDescent="0.35">
       <c r="A6" s="5"/>
       <c r="B6" s="5" t="str">
         <f t="shared" ref="B6:B69" si="2">IF(A6="","",SUM(D6:BA6))</f>
@@ -7591,7 +7603,7 @@
       <c r="AZ6" s="9"/>
       <c r="BA6" s="9"/>
     </row>
-    <row r="7" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:53" x14ac:dyDescent="0.35">
       <c r="A7" s="5"/>
       <c r="B7" s="5" t="str">
         <f t="shared" si="2"/>
@@ -7622,7 +7634,7 @@
       <c r="V7" s="9"/>
       <c r="W7" s="9"/>
     </row>
-    <row r="8" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:53" x14ac:dyDescent="0.35">
       <c r="A8" s="5"/>
       <c r="B8" s="5" t="str">
         <f t="shared" si="2"/>
@@ -7653,7 +7665,7 @@
       <c r="V8" s="9"/>
       <c r="W8" s="9"/>
     </row>
-    <row r="9" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:53" x14ac:dyDescent="0.35">
       <c r="A9" s="5"/>
       <c r="B9" s="5" t="str">
         <f t="shared" si="2"/>
@@ -7684,7 +7696,7 @@
       <c r="V9" s="9"/>
       <c r="W9" s="9"/>
     </row>
-    <row r="10" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:53" x14ac:dyDescent="0.35">
       <c r="A10" s="5"/>
       <c r="B10" s="5" t="str">
         <f t="shared" si="2"/>
@@ -7715,7 +7727,7 @@
       <c r="V10" s="9"/>
       <c r="W10" s="9"/>
     </row>
-    <row r="11" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:53" x14ac:dyDescent="0.35">
       <c r="A11" s="5"/>
       <c r="B11" s="5" t="str">
         <f t="shared" si="2"/>
@@ -7746,7 +7758,7 @@
       <c r="V11" s="9"/>
       <c r="W11" s="9"/>
     </row>
-    <row r="12" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:53" x14ac:dyDescent="0.35">
       <c r="A12" s="5"/>
       <c r="B12" s="5" t="str">
         <f t="shared" si="2"/>
@@ -7777,7 +7789,7 @@
       <c r="V12" s="9"/>
       <c r="W12" s="9"/>
     </row>
-    <row r="13" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:53" x14ac:dyDescent="0.35">
       <c r="A13" s="5"/>
       <c r="B13" s="5" t="str">
         <f t="shared" si="2"/>
@@ -7808,7 +7820,7 @@
       <c r="V13" s="9"/>
       <c r="W13" s="9"/>
     </row>
-    <row r="14" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:53" x14ac:dyDescent="0.35">
       <c r="A14" s="5"/>
       <c r="B14" s="5" t="str">
         <f t="shared" si="2"/>
@@ -7839,7 +7851,7 @@
       <c r="V14" s="9"/>
       <c r="W14" s="9"/>
     </row>
-    <row r="15" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:53" x14ac:dyDescent="0.35">
       <c r="A15" s="5"/>
       <c r="B15" s="5" t="str">
         <f t="shared" si="2"/>
@@ -7870,7 +7882,7 @@
       <c r="V15" s="9"/>
       <c r="W15" s="9"/>
     </row>
-    <row r="16" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:53" x14ac:dyDescent="0.35">
       <c r="A16" s="5"/>
       <c r="B16" s="5" t="str">
         <f t="shared" si="2"/>
@@ -7901,7 +7913,7 @@
       <c r="V16" s="9"/>
       <c r="W16" s="9"/>
     </row>
-    <row r="17" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A17" s="5"/>
       <c r="B17" s="5" t="str">
         <f t="shared" si="2"/>
@@ -7932,7 +7944,7 @@
       <c r="V17" s="9"/>
       <c r="W17" s="9"/>
     </row>
-    <row r="18" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A18" s="5"/>
       <c r="B18" s="5" t="str">
         <f t="shared" si="2"/>
@@ -7963,7 +7975,7 @@
       <c r="V18" s="9"/>
       <c r="W18" s="9"/>
     </row>
-    <row r="19" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A19" s="5"/>
       <c r="B19" s="5" t="str">
         <f t="shared" si="2"/>
@@ -7994,7 +8006,7 @@
       <c r="V19" s="9"/>
       <c r="W19" s="9"/>
     </row>
-    <row r="20" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A20" s="5"/>
       <c r="B20" s="5" t="str">
         <f t="shared" si="2"/>
@@ -8025,7 +8037,7 @@
       <c r="V20" s="9"/>
       <c r="W20" s="9"/>
     </row>
-    <row r="21" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A21" s="5"/>
       <c r="B21" s="5" t="str">
         <f t="shared" si="2"/>
@@ -8056,7 +8068,7 @@
       <c r="V21" s="9"/>
       <c r="W21" s="9"/>
     </row>
-    <row r="22" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A22" s="5"/>
       <c r="B22" s="5" t="str">
         <f t="shared" si="2"/>
@@ -8087,7 +8099,7 @@
       <c r="V22" s="9"/>
       <c r="W22" s="9"/>
     </row>
-    <row r="23" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A23" s="5"/>
       <c r="B23" s="5" t="str">
         <f t="shared" si="2"/>
@@ -8118,7 +8130,7 @@
       <c r="V23" s="9"/>
       <c r="W23" s="9"/>
     </row>
-    <row r="24" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A24" s="5"/>
       <c r="B24" s="5" t="str">
         <f t="shared" si="2"/>
@@ -8149,7 +8161,7 @@
       <c r="V24" s="9"/>
       <c r="W24" s="9"/>
     </row>
-    <row r="25" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A25" s="5"/>
       <c r="B25" s="5" t="str">
         <f t="shared" si="2"/>
@@ -8180,7 +8192,7 @@
       <c r="V25" s="9"/>
       <c r="W25" s="9"/>
     </row>
-    <row r="26" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A26" s="5"/>
       <c r="B26" s="5" t="str">
         <f t="shared" si="2"/>
@@ -8211,7 +8223,7 @@
       <c r="V26" s="9"/>
       <c r="W26" s="9"/>
     </row>
-    <row r="27" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A27" s="5"/>
       <c r="B27" s="5" t="str">
         <f t="shared" si="2"/>
@@ -8242,7 +8254,7 @@
       <c r="V27" s="9"/>
       <c r="W27" s="9"/>
     </row>
-    <row r="28" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A28" s="5"/>
       <c r="B28" s="5" t="str">
         <f t="shared" si="2"/>
@@ -8273,7 +8285,7 @@
       <c r="V28" s="9"/>
       <c r="W28" s="9"/>
     </row>
-    <row r="29" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A29" s="5"/>
       <c r="B29" s="5" t="str">
         <f t="shared" si="2"/>
@@ -8304,7 +8316,7 @@
       <c r="V29" s="9"/>
       <c r="W29" s="9"/>
     </row>
-    <row r="30" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A30" s="5"/>
       <c r="B30" s="5" t="str">
         <f t="shared" si="2"/>
@@ -8335,7 +8347,7 @@
       <c r="V30" s="9"/>
       <c r="W30" s="9"/>
     </row>
-    <row r="31" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A31" s="5"/>
       <c r="B31" s="5" t="str">
         <f t="shared" si="2"/>
@@ -8366,7 +8378,7 @@
       <c r="V31" s="9"/>
       <c r="W31" s="9"/>
     </row>
-    <row r="32" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A32" s="5"/>
       <c r="B32" s="5" t="str">
         <f t="shared" si="2"/>
@@ -8397,7 +8409,7 @@
       <c r="V32" s="9"/>
       <c r="W32" s="9"/>
     </row>
-    <row r="33" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A33" s="5"/>
       <c r="B33" s="5" t="str">
         <f t="shared" si="2"/>
@@ -8428,7 +8440,7 @@
       <c r="V33" s="9"/>
       <c r="W33" s="9"/>
     </row>
-    <row r="34" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A34" s="5"/>
       <c r="B34" s="5" t="str">
         <f t="shared" si="2"/>
@@ -8459,7 +8471,7 @@
       <c r="V34" s="9"/>
       <c r="W34" s="9"/>
     </row>
-    <row r="35" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A35" s="5"/>
       <c r="B35" s="5" t="str">
         <f t="shared" si="2"/>
@@ -8490,7 +8502,7 @@
       <c r="V35" s="9"/>
       <c r="W35" s="9"/>
     </row>
-    <row r="36" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A36" s="5"/>
       <c r="B36" s="5" t="str">
         <f t="shared" si="2"/>
@@ -8521,7 +8533,7 @@
       <c r="V36" s="9"/>
       <c r="W36" s="9"/>
     </row>
-    <row r="37" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A37" s="5"/>
       <c r="B37" s="5" t="str">
         <f t="shared" si="2"/>
@@ -8552,7 +8564,7 @@
       <c r="V37" s="9"/>
       <c r="W37" s="9"/>
     </row>
-    <row r="38" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A38" s="5"/>
       <c r="B38" s="5" t="str">
         <f t="shared" si="2"/>
@@ -8583,7 +8595,7 @@
       <c r="V38" s="9"/>
       <c r="W38" s="9"/>
     </row>
-    <row r="39" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A39" s="5"/>
       <c r="B39" s="5" t="str">
         <f t="shared" si="2"/>
@@ -8614,7 +8626,7 @@
       <c r="V39" s="9"/>
       <c r="W39" s="9"/>
     </row>
-    <row r="40" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A40" s="5"/>
       <c r="B40" s="5" t="str">
         <f t="shared" si="2"/>
@@ -8645,7 +8657,7 @@
       <c r="V40" s="9"/>
       <c r="W40" s="9"/>
     </row>
-    <row r="41" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A41" s="5"/>
       <c r="B41" s="5" t="str">
         <f t="shared" si="2"/>
@@ -8676,7 +8688,7 @@
       <c r="V41" s="9"/>
       <c r="W41" s="9"/>
     </row>
-    <row r="42" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A42" s="5"/>
       <c r="B42" s="5" t="str">
         <f t="shared" si="2"/>
@@ -8707,7 +8719,7 @@
       <c r="V42" s="9"/>
       <c r="W42" s="9"/>
     </row>
-    <row r="43" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A43" s="5"/>
       <c r="B43" s="5" t="str">
         <f t="shared" si="2"/>
@@ -8738,7 +8750,7 @@
       <c r="V43" s="9"/>
       <c r="W43" s="9"/>
     </row>
-    <row r="44" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A44" s="5"/>
       <c r="B44" s="5" t="str">
         <f t="shared" si="2"/>
@@ -8769,7 +8781,7 @@
       <c r="V44" s="9"/>
       <c r="W44" s="9"/>
     </row>
-    <row r="45" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A45" s="5"/>
       <c r="B45" s="5" t="str">
         <f t="shared" si="2"/>
@@ -8800,7 +8812,7 @@
       <c r="V45" s="9"/>
       <c r="W45" s="9"/>
     </row>
-    <row r="46" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A46" s="5"/>
       <c r="B46" s="5" t="str">
         <f t="shared" si="2"/>
@@ -8831,7 +8843,7 @@
       <c r="V46" s="9"/>
       <c r="W46" s="9"/>
     </row>
-    <row r="47" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A47" s="5"/>
       <c r="B47" s="5" t="str">
         <f t="shared" si="2"/>
@@ -8862,7 +8874,7 @@
       <c r="V47" s="9"/>
       <c r="W47" s="9"/>
     </row>
-    <row r="48" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A48" s="5"/>
       <c r="B48" s="5" t="str">
         <f t="shared" si="2"/>
@@ -8893,7 +8905,7 @@
       <c r="V48" s="9"/>
       <c r="W48" s="9"/>
     </row>
-    <row r="49" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A49" s="5"/>
       <c r="B49" s="5" t="str">
         <f t="shared" si="2"/>
@@ -8924,7 +8936,7 @@
       <c r="V49" s="9"/>
       <c r="W49" s="9"/>
     </row>
-    <row r="50" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A50" s="5"/>
       <c r="B50" s="5" t="str">
         <f t="shared" si="2"/>
@@ -8955,7 +8967,7 @@
       <c r="V50" s="9"/>
       <c r="W50" s="9"/>
     </row>
-    <row r="51" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A51" s="5"/>
       <c r="B51" s="5" t="str">
         <f t="shared" si="2"/>
@@ -8986,7 +8998,7 @@
       <c r="V51" s="9"/>
       <c r="W51" s="9"/>
     </row>
-    <row r="52" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A52" s="5"/>
       <c r="B52" s="5" t="str">
         <f t="shared" si="2"/>
@@ -9017,7 +9029,7 @@
       <c r="V52" s="9"/>
       <c r="W52" s="9"/>
     </row>
-    <row r="53" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A53" s="5"/>
       <c r="B53" s="5" t="str">
         <f t="shared" si="2"/>
@@ -9048,7 +9060,7 @@
       <c r="V53" s="9"/>
       <c r="W53" s="9"/>
     </row>
-    <row r="54" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A54" s="5"/>
       <c r="B54" s="5" t="str">
         <f t="shared" si="2"/>
@@ -9079,7 +9091,7 @@
       <c r="V54" s="9"/>
       <c r="W54" s="9"/>
     </row>
-    <row r="55" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A55" s="5"/>
       <c r="B55" s="5" t="str">
         <f t="shared" si="2"/>
@@ -9110,7 +9122,7 @@
       <c r="V55" s="9"/>
       <c r="W55" s="9"/>
     </row>
-    <row r="56" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A56" s="5"/>
       <c r="B56" s="5" t="str">
         <f t="shared" si="2"/>
@@ -9141,7 +9153,7 @@
       <c r="V56" s="9"/>
       <c r="W56" s="9"/>
     </row>
-    <row r="57" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A57" s="5"/>
       <c r="B57" s="5" t="str">
         <f t="shared" si="2"/>
@@ -9172,7 +9184,7 @@
       <c r="V57" s="9"/>
       <c r="W57" s="9"/>
     </row>
-    <row r="58" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A58" s="5"/>
       <c r="B58" s="5" t="str">
         <f t="shared" si="2"/>
@@ -9203,7 +9215,7 @@
       <c r="V58" s="9"/>
       <c r="W58" s="9"/>
     </row>
-    <row r="59" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A59" s="5"/>
       <c r="B59" s="5" t="str">
         <f t="shared" si="2"/>
@@ -9234,7 +9246,7 @@
       <c r="V59" s="9"/>
       <c r="W59" s="9"/>
     </row>
-    <row r="60" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A60" s="5"/>
       <c r="B60" s="5" t="str">
         <f t="shared" si="2"/>
@@ -9265,7 +9277,7 @@
       <c r="V60" s="9"/>
       <c r="W60" s="9"/>
     </row>
-    <row r="61" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A61" s="5"/>
       <c r="B61" s="5" t="str">
         <f t="shared" si="2"/>
@@ -9296,7 +9308,7 @@
       <c r="V61" s="9"/>
       <c r="W61" s="9"/>
     </row>
-    <row r="62" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A62" s="5"/>
       <c r="B62" s="5" t="str">
         <f t="shared" si="2"/>
@@ -9327,7 +9339,7 @@
       <c r="V62" s="9"/>
       <c r="W62" s="9"/>
     </row>
-    <row r="63" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A63" s="5"/>
       <c r="B63" s="5" t="str">
         <f t="shared" si="2"/>
@@ -9358,7 +9370,7 @@
       <c r="V63" s="9"/>
       <c r="W63" s="9"/>
     </row>
-    <row r="64" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A64" s="5"/>
       <c r="B64" s="5" t="str">
         <f t="shared" si="2"/>
@@ -9389,7 +9401,7 @@
       <c r="V64" s="9"/>
       <c r="W64" s="9"/>
     </row>
-    <row r="65" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A65" s="5"/>
       <c r="B65" s="5" t="str">
         <f t="shared" si="2"/>
@@ -9420,7 +9432,7 @@
       <c r="V65" s="9"/>
       <c r="W65" s="9"/>
     </row>
-    <row r="66" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A66" s="5"/>
       <c r="B66" s="5" t="str">
         <f t="shared" si="2"/>
@@ -9451,7 +9463,7 @@
       <c r="V66" s="9"/>
       <c r="W66" s="9"/>
     </row>
-    <row r="67" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A67" s="5"/>
       <c r="B67" s="5" t="str">
         <f t="shared" si="2"/>
@@ -9482,7 +9494,7 @@
       <c r="V67" s="9"/>
       <c r="W67" s="9"/>
     </row>
-    <row r="68" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A68" s="5"/>
       <c r="B68" s="5" t="str">
         <f t="shared" si="2"/>
@@ -9513,7 +9525,7 @@
       <c r="V68" s="9"/>
       <c r="W68" s="9"/>
     </row>
-    <row r="69" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A69" s="5"/>
       <c r="B69" s="5" t="str">
         <f t="shared" si="2"/>
@@ -9544,7 +9556,7 @@
       <c r="V69" s="9"/>
       <c r="W69" s="9"/>
     </row>
-    <row r="70" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A70" s="5"/>
       <c r="B70" s="5" t="str">
         <f t="shared" ref="B70:B81" si="4">IF(A70="","",SUM(D70:BA70))</f>
@@ -9555,7 +9567,7 @@
         <v/>
       </c>
     </row>
-    <row r="71" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A71" s="5"/>
       <c r="B71" s="5" t="str">
         <f t="shared" si="4"/>
@@ -9566,7 +9578,7 @@
         <v/>
       </c>
     </row>
-    <row r="72" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A72" s="5"/>
       <c r="B72" s="5" t="str">
         <f t="shared" si="4"/>
@@ -9577,7 +9589,7 @@
         <v/>
       </c>
     </row>
-    <row r="73" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A73" s="5"/>
       <c r="B73" s="5" t="str">
         <f t="shared" si="4"/>
@@ -9588,7 +9600,7 @@
         <v/>
       </c>
     </row>
-    <row r="74" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A74" s="5"/>
       <c r="B74" s="5" t="str">
         <f t="shared" si="4"/>
@@ -9599,7 +9611,7 @@
         <v/>
       </c>
     </row>
-    <row r="75" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A75" s="5"/>
       <c r="B75" s="5" t="str">
         <f t="shared" si="4"/>
@@ -9610,7 +9622,7 @@
         <v/>
       </c>
     </row>
-    <row r="76" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A76" s="5"/>
       <c r="B76" s="5" t="str">
         <f t="shared" si="4"/>
@@ -9621,7 +9633,7 @@
         <v/>
       </c>
     </row>
-    <row r="77" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A77" s="5"/>
       <c r="B77" s="5" t="str">
         <f t="shared" si="4"/>
@@ -9632,7 +9644,7 @@
         <v/>
       </c>
     </row>
-    <row r="78" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A78" s="5"/>
       <c r="B78" s="5" t="str">
         <f t="shared" si="4"/>
@@ -9643,7 +9655,7 @@
         <v/>
       </c>
     </row>
-    <row r="79" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A79" s="5"/>
       <c r="B79" s="5" t="str">
         <f t="shared" si="4"/>
@@ -9654,7 +9666,7 @@
         <v/>
       </c>
     </row>
-    <row r="80" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A80" s="5"/>
       <c r="B80" s="5" t="str">
         <f t="shared" si="4"/>
@@ -9665,7 +9677,7 @@
         <v/>
       </c>
     </row>
-    <row r="81" spans="1:97" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:97" x14ac:dyDescent="0.35">
       <c r="A81" s="5"/>
       <c r="B81" s="5" t="str">
         <f t="shared" si="4"/>
@@ -9676,13 +9688,13 @@
         <v/>
       </c>
     </row>
-    <row r="82" spans="1:97" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:97" x14ac:dyDescent="0.35">
       <c r="C82" s="8" t="str">
         <f t="shared" si="5"/>
         <v/>
       </c>
     </row>
-    <row r="83" spans="1:97" hidden="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:97" hidden="1" x14ac:dyDescent="0.35">
       <c r="A83" s="1" t="s">
         <v>11</v>
       </c>
@@ -10065,12 +10077,12 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A6:A90 D5:CD5">
-    <cfRule type="notContainsBlanks" dxfId="1" priority="2">
+    <cfRule type="notContainsBlanks" dxfId="2" priority="2">
       <formula>LEN(TRIM(A5))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B6:C88">
-    <cfRule type="notContainsBlanks" dxfId="0" priority="1">
+    <cfRule type="notContainsBlanks" dxfId="1" priority="1">
       <formula>LEN(TRIM(B6))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -10087,12 +10099,12 @@
       <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="5" width="13.42578125"/>
+    <col min="1" max="5" width="13.453125"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="10" t="s">
         <v>7</v>
       </c>

</xml_diff>